<commit_message>
added speed up in excel files
</commit_message>
<xml_diff>
--- a/time_2070.xlsx
+++ b/time_2070.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7032"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7032"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
   <si>
     <t>standard memory</t>
   </si>
@@ -65,7 +65,13 @@
     <t>08x08</t>
   </si>
   <si>
-    <t>speed_up</t>
+    <t>speed_up_tot</t>
+  </si>
+  <si>
+    <t>speed_up_init</t>
+  </si>
+  <si>
+    <t>speed_up_add</t>
   </si>
 </sst>
 </file>
@@ -73,8 +79,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -113,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -122,22 +128,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -156,21 +175,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:G13" totalsRowShown="0">
-  <autoFilter ref="A1:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:I13" totalsRowShown="0">
+  <autoFilter ref="A1:I13"/>
   <sortState ref="A2:F13">
     <sortCondition ref="A1:A13"/>
   </sortState>
-  <tableColumns count="7">
+  <tableColumns count="9">
     <tableColumn id="1" name="mem_type"/>
     <tableColumn id="2" name="kernel_type"/>
-    <tableColumn id="3" name="dim_grid" dataDxfId="3"/>
-    <tableColumn id="4" name="init_min_time" dataDxfId="2"/>
-    <tableColumn id="5" name="add_min_time" dataDxfId="1"/>
-    <tableColumn id="6" name="total_time" dataDxfId="0">
+    <tableColumn id="3" name="dim_grid" dataDxfId="6"/>
+    <tableColumn id="4" name="init_min_time" dataDxfId="5"/>
+    <tableColumn id="5" name="add_min_time" dataDxfId="4"/>
+    <tableColumn id="6" name="total_time" dataDxfId="3">
       <calculatedColumnFormula>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="speed_up"/>
+    <tableColumn id="7" name="speed_up_init" dataDxfId="2">
+      <calculatedColumnFormula>1278/Tabella1[[#This Row],[init_min_time]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="speed_up_add" dataDxfId="1">
+      <calculatedColumnFormula>294/Tabella1[[#This Row],[add_min_time]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="speed_up_tot" dataDxfId="0">
+      <calculatedColumnFormula>1572/Tabella1[[#This Row],[total_time]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -442,7 +469,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G1" sqref="G1:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,8 +478,10 @@
     <col min="2" max="2" width="17.5546875" customWidth="1"/>
     <col min="3" max="3" width="10.88671875" customWidth="1"/>
     <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="5" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -475,6 +504,12 @@
         <v>9</v>
       </c>
       <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -498,6 +533,18 @@
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
         <v>11.086300000000001</v>
       </c>
+      <c r="G2" s="7">
+        <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
+        <v>470.5275947130076</v>
+      </c>
+      <c r="H2" s="7">
+        <f>294/Tabella1[[#This Row],[add_min_time]]</f>
+        <v>35.124608730974167</v>
+      </c>
+      <c r="I2" s="7">
+        <f>1572/Tabella1[[#This Row],[total_time]]</f>
+        <v>141.79663187898575</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -519,6 +566,18 @@
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
         <v>11.099799999999998</v>
       </c>
+      <c r="G3" s="7">
+        <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
+        <v>470.5275947130076</v>
+      </c>
+      <c r="H3" s="7">
+        <f>294/Tabella1[[#This Row],[add_min_time]]</f>
+        <v>35.068048713575152</v>
+      </c>
+      <c r="I3" s="7">
+        <f>1572/Tabella1[[#This Row],[total_time]]</f>
+        <v>141.62417340852991</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -540,6 +599,18 @@
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
         <v>12.5412</v>
       </c>
+      <c r="G4" s="7">
+        <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
+        <v>384.41870958038805</v>
+      </c>
+      <c r="H4" s="7">
+        <f>294/Tabella1[[#This Row],[add_min_time]]</f>
+        <v>31.898618811505205</v>
+      </c>
+      <c r="I4" s="7">
+        <f>1572/Tabella1[[#This Row],[total_time]]</f>
+        <v>125.34685676011865</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -561,6 +632,18 @@
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
         <v>10.897500000000001</v>
       </c>
+      <c r="G5" s="7">
+        <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
+        <v>462.72493573264785</v>
+      </c>
+      <c r="H5" s="7">
+        <f>294/Tabella1[[#This Row],[add_min_time]]</f>
+        <v>36.13746988544176</v>
+      </c>
+      <c r="I5" s="7">
+        <f>1572/Tabella1[[#This Row],[total_time]]</f>
+        <v>144.25326909841706</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -582,6 +665,18 @@
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
         <v>10.9313</v>
       </c>
+      <c r="G6" s="7">
+        <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
+        <v>449.46191179573754</v>
+      </c>
+      <c r="H6" s="7">
+        <f>294/Tabella1[[#This Row],[add_min_time]]</f>
+        <v>36.350597806599986</v>
+      </c>
+      <c r="I6" s="7">
+        <f>1572/Tabella1[[#This Row],[total_time]]</f>
+        <v>143.8072324426189</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -603,6 +698,18 @@
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
         <v>11.119100000000001</v>
       </c>
+      <c r="G7" s="7">
+        <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
+        <v>446.80627906163687</v>
+      </c>
+      <c r="H7" s="7">
+        <f>294/Tabella1[[#This Row],[add_min_time]]</f>
+        <v>35.598392018210873</v>
+      </c>
+      <c r="I7" s="7">
+        <f>1572/Tabella1[[#This Row],[total_time]]</f>
+        <v>141.37834896709265</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -624,6 +731,18 @@
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
         <v>11.039100000000001</v>
       </c>
+      <c r="G8" s="7">
+        <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
+        <v>465.55681031656405</v>
+      </c>
+      <c r="H8" s="7">
+        <f>294/Tabella1[[#This Row],[add_min_time]]</f>
+        <v>35.447311309380275</v>
+      </c>
+      <c r="I8" s="7">
+        <f>1572/Tabella1[[#This Row],[total_time]]</f>
+        <v>142.40291328097396</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -645,6 +764,18 @@
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
         <v>10.938400000000001</v>
       </c>
+      <c r="G9" s="7">
+        <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
+        <v>443.5190005205622</v>
+      </c>
+      <c r="H9" s="7">
+        <f>294/Tabella1[[#This Row],[add_min_time]]</f>
+        <v>36.490461591927414</v>
+      </c>
+      <c r="I9" s="7">
+        <f>1572/Tabella1[[#This Row],[total_time]]</f>
+        <v>143.71388868573098</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -666,7 +797,18 @@
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
         <v>13.4315</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="G10" s="7">
+        <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
+        <v>356.24686402408429</v>
+      </c>
+      <c r="H10" s="7">
+        <f>294/Tabella1[[#This Row],[add_min_time]]</f>
+        <v>29.865604778496767</v>
+      </c>
+      <c r="I10" s="8">
+        <f>1572/Tabella1[[#This Row],[total_time]]</f>
+        <v>117.03830547593344</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -688,6 +830,18 @@
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
         <v>10.953199999999999</v>
       </c>
+      <c r="G11" s="7">
+        <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
+        <v>474.91638795986626</v>
+      </c>
+      <c r="H11" s="7">
+        <f>294/Tabella1[[#This Row],[add_min_time]]</f>
+        <v>35.583742828786519</v>
+      </c>
+      <c r="I11" s="7">
+        <f>1572/Tabella1[[#This Row],[total_time]]</f>
+        <v>143.51970200489356</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -709,6 +863,18 @@
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
         <v>11.897500000000001</v>
       </c>
+      <c r="G12" s="7">
+        <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
+        <v>435.80562659846544</v>
+      </c>
+      <c r="H12" s="7">
+        <f>294/Tabella1[[#This Row],[add_min_time]]</f>
+        <v>32.794199665365312</v>
+      </c>
+      <c r="I12" s="7">
+        <f>1572/Tabella1[[#This Row],[total_time]]</f>
+        <v>132.12859844505147</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -729,6 +895,18 @@
       <c r="F13" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
         <v>10.923399999999999</v>
+      </c>
+      <c r="G13" s="7">
+        <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
+        <v>444.84667061157717</v>
+      </c>
+      <c r="H13" s="7">
+        <f>294/Tabella1[[#This Row],[add_min_time]]</f>
+        <v>36.51947084032048</v>
+      </c>
+      <c r="I13" s="7">
+        <f>1572/Tabella1[[#This Row],[total_time]]</f>
+        <v>143.91123642821833</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>